<commit_message>
dev: update test oids
</commit_message>
<xml_diff>
--- a/test/data/test-snmp3-oids-sheet.xlsx
+++ b/test/data/test-snmp3-oids-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>oid</t>
   </si>
@@ -41,31 +41,445 @@
     <t>frequency</t>
   </si>
   <si>
-    <t>.1.3.6.1.2.1.1.1.0</t>
-  </si>
-  <si>
-    <t>Total Processes</t>
-  </si>
-  <si>
-    <t>线程总数</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.2.1.1.5.0</t>
-  </si>
-  <si>
-    <t>Users Count</t>
-  </si>
-  <si>
-    <t>用户总数</t>
-  </si>
-  <si>
-    <t>.1.3.6.1.2.1.1.7.0</t>
-  </si>
-  <si>
-    <t>CPU</t>
-  </si>
-  <si>
-    <t>CPU使用率</t>
+    <t>1.3.6.1.2.1.1.1</t>
+  </si>
+  <si>
+    <t>sysDescr</t>
+  </si>
+  <si>
+    <t>描述系统的信息</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.1.2</t>
+  </si>
+  <si>
+    <t>sysObjectID</t>
+  </si>
+  <si>
+    <t>引用系统的身份信息</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.1.3</t>
+  </si>
+  <si>
+    <t>sysUpTime</t>
+  </si>
+  <si>
+    <t>系统运行时间</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.1.4</t>
+  </si>
+  <si>
+    <t>sysContact</t>
+  </si>
+  <si>
+    <t>系统管理员的联系方式</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.1.5</t>
+  </si>
+  <si>
+    <t>sysName</t>
+  </si>
+  <si>
+    <t>系统的名称</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.1.6</t>
+  </si>
+  <si>
+    <t>sysLocation</t>
+  </si>
+  <si>
+    <t>系统的位置信息</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.1</t>
+  </si>
+  <si>
+    <t>ifNumber</t>
+  </si>
+  <si>
+    <t>接口的数量</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2</t>
+  </si>
+  <si>
+    <t>ifTable</t>
+  </si>
+  <si>
+    <t>接口的信息表</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.1</t>
+  </si>
+  <si>
+    <t>ifIndex</t>
+  </si>
+  <si>
+    <t>接口的索引</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.2</t>
+  </si>
+  <si>
+    <t>ifDescr</t>
+  </si>
+  <si>
+    <t>接口的描述</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.3</t>
+  </si>
+  <si>
+    <t>ifType</t>
+  </si>
+  <si>
+    <t>接口的类型</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.4</t>
+  </si>
+  <si>
+    <t>ifMtu</t>
+  </si>
+  <si>
+    <t>接口的最大传输单元</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.5</t>
+  </si>
+  <si>
+    <t>ifSpeed</t>
+  </si>
+  <si>
+    <t>接口的速率</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.6</t>
+  </si>
+  <si>
+    <t>ifPhysAddress</t>
+  </si>
+  <si>
+    <t>接口的物理地址</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.7</t>
+  </si>
+  <si>
+    <t>ifAdminStatus</t>
+  </si>
+  <si>
+    <t>接口的管理状态</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.8</t>
+  </si>
+  <si>
+    <t>ifOperStatus</t>
+  </si>
+  <si>
+    <t>接口的操作状态</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.9</t>
+  </si>
+  <si>
+    <t>ifLastChange</t>
+  </si>
+  <si>
+    <t>接口的最后修改时间</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.10</t>
+  </si>
+  <si>
+    <t>ifInOctets</t>
+  </si>
+  <si>
+    <t>接口接收的字节数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.11</t>
+  </si>
+  <si>
+    <t>ifInUcastPkts</t>
+  </si>
+  <si>
+    <t>接口接收的单播数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.12</t>
+  </si>
+  <si>
+    <t>ifInNUcastPkts</t>
+  </si>
+  <si>
+    <t>接口接收的非单播数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.13</t>
+  </si>
+  <si>
+    <t>ifInDiscards</t>
+  </si>
+  <si>
+    <t>接口接收的丢弃数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.14</t>
+  </si>
+  <si>
+    <t>ifInErrors</t>
+  </si>
+  <si>
+    <t>接口接收的错误数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.15</t>
+  </si>
+  <si>
+    <t>ifInUnknownProtos</t>
+  </si>
+  <si>
+    <t>接口接收的未知协议数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.16</t>
+  </si>
+  <si>
+    <t>ifOutOctets</t>
+  </si>
+  <si>
+    <t>接口发送的字节数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.17</t>
+  </si>
+  <si>
+    <t>ifOutUcastPkts</t>
+  </si>
+  <si>
+    <t>接口发送的单播数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.18</t>
+  </si>
+  <si>
+    <t>ifOutNUcastPkts</t>
+  </si>
+  <si>
+    <t>接口发送的非单播数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.19</t>
+  </si>
+  <si>
+    <t>ifOutDiscards</t>
+  </si>
+  <si>
+    <t>接口发送的丢弃数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.20</t>
+  </si>
+  <si>
+    <t>ifOutErrors</t>
+  </si>
+  <si>
+    <t>接口发送的错误数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.2.2.1.21</t>
+  </si>
+  <si>
+    <t>ifOutQLen</t>
+  </si>
+  <si>
+    <t>接口发送队列的长度</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.1</t>
+  </si>
+  <si>
+    <t>ipForwarding</t>
+  </si>
+  <si>
+    <t>IP 转发表的状态</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.2</t>
+  </si>
+  <si>
+    <t>ipDefaultTTL</t>
+  </si>
+  <si>
+    <t>IP 数据包的默认 TTL</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.3</t>
+  </si>
+  <si>
+    <t>ipInReceives</t>
+  </si>
+  <si>
+    <t>接收的 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.4</t>
+  </si>
+  <si>
+    <t>ipInHdrErrors</t>
+  </si>
+  <si>
+    <t>接收的 IP 包头错误数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.5</t>
+  </si>
+  <si>
+    <t>ipInAddrErrors</t>
+  </si>
+  <si>
+    <t>接收的 IP 地址错误数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.6</t>
+  </si>
+  <si>
+    <t>ipForwDatagrams</t>
+  </si>
+  <si>
+    <t>转发的 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.7</t>
+  </si>
+  <si>
+    <t>ipInUnknownProtos</t>
+  </si>
+  <si>
+    <t>接收的未知协议 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.8</t>
+  </si>
+  <si>
+    <t>ipInDiscards</t>
+  </si>
+  <si>
+    <t>接收的丢弃 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.9</t>
+  </si>
+  <si>
+    <t>ipInDelivers</t>
+  </si>
+  <si>
+    <t>接收并送达的 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.10</t>
+  </si>
+  <si>
+    <t>ipOutRequests</t>
+  </si>
+  <si>
+    <t>发送的 IP 请求包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.11</t>
+  </si>
+  <si>
+    <t>ipOutDiscards</t>
+  </si>
+  <si>
+    <t>发送的丢弃 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.12</t>
+  </si>
+  <si>
+    <t>ipOutNoRoutes</t>
+  </si>
+  <si>
+    <t>发送的无路由 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.13</t>
+  </si>
+  <si>
+    <t>ipReasmTimeout</t>
+  </si>
+  <si>
+    <t>IP 数据包重组超时数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.14</t>
+  </si>
+  <si>
+    <t>ipReasmReqds</t>
+  </si>
+  <si>
+    <t>IP 数据包重组请求数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.15</t>
+  </si>
+  <si>
+    <t>ipReasmOKs</t>
+  </si>
+  <si>
+    <t>成功重组的 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.16</t>
+  </si>
+  <si>
+    <t>ipReasmFails</t>
+  </si>
+  <si>
+    <t>重组失败的 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.17</t>
+  </si>
+  <si>
+    <t>ipFragOKs</t>
+  </si>
+  <si>
+    <t>成功分段的 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.18</t>
+  </si>
+  <si>
+    <t>ipFragFails</t>
+  </si>
+  <si>
+    <t>分段失败的 IP 数据包数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.3.1.19</t>
+  </si>
+  <si>
+    <t>ipFragCreates</t>
+  </si>
+  <si>
+    <t>创建的 IP 数据包分段数</t>
+  </si>
+  <si>
+    <t>1.3.6.1.2.1.4.1</t>
+  </si>
+  <si>
+    <t>icmpInMsgs</t>
+  </si>
+  <si>
+    <t>接收的 ICMP 消息数</t>
   </si>
 </sst>
 </file>
@@ -78,7 +492,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,12 +507,6 @@
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF24292F"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -586,133 +994,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -726,7 +1134,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1254,17 +1662,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A5" sqref="$A5:$XFD5"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="28.525" customWidth="1"/>
-    <col min="2" max="2" width="16.525" customWidth="1"/>
-    <col min="4" max="4" width="13.6916666666667" customWidth="1"/>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1"/>
+    <col min="3" max="3" width="27.75" customWidth="1"/>
+    <col min="4" max="4" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" spans="1:4">
@@ -1281,46 +1690,690 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:4">
+      <c r="D2" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
+      <c r="B34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dev: enhance snmp module
</commit_message>
<xml_diff>
--- a/test/data/test-snmp3-oids-sheet.xlsx
+++ b/test/data/test-snmp3-oids-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>oid</t>
   </si>
@@ -41,445 +41,67 @@
     <t>frequency</t>
   </si>
   <si>
-    <t>1.3.6.1.2.1.1.1</t>
-  </si>
-  <si>
-    <t>sysDescr</t>
-  </si>
-  <si>
-    <t>描述系统的信息</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.1.2</t>
-  </si>
-  <si>
-    <t>sysObjectID</t>
-  </si>
-  <si>
-    <t>引用系统的身份信息</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.1.3</t>
-  </si>
-  <si>
-    <t>sysUpTime</t>
-  </si>
-  <si>
-    <t>系统运行时间</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.1.4</t>
+    <t>.1.3.6.1.2.1.1.1.0</t>
+  </si>
+  <si>
+    <t>获取系统基本信息</t>
+  </si>
+  <si>
+    <t>SysDesc</t>
+  </si>
+  <si>
+    <t>.1.3.6.1.2.1.1.3.0</t>
+  </si>
+  <si>
+    <t>监控时间</t>
+  </si>
+  <si>
+    <t>sysUptime</t>
+  </si>
+  <si>
+    <t>.1.3.6.1.2.1.1.4.0</t>
+  </si>
+  <si>
+    <t>系统联系人</t>
   </si>
   <si>
     <t>sysContact</t>
   </si>
   <si>
-    <t>系统管理员的联系方式</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.1.5</t>
-  </si>
-  <si>
-    <t>sysName</t>
-  </si>
-  <si>
-    <t>系统的名称</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.1.6</t>
-  </si>
-  <si>
-    <t>sysLocation</t>
-  </si>
-  <si>
-    <t>系统的位置信息</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.1</t>
-  </si>
-  <si>
-    <t>ifNumber</t>
-  </si>
-  <si>
-    <t>接口的数量</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2</t>
-  </si>
-  <si>
-    <t>ifTable</t>
-  </si>
-  <si>
-    <t>接口的信息表</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.1</t>
-  </si>
-  <si>
-    <t>ifIndex</t>
-  </si>
-  <si>
-    <t>接口的索引</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.2</t>
-  </si>
-  <si>
-    <t>ifDescr</t>
-  </si>
-  <si>
-    <t>接口的描述</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.3</t>
-  </si>
-  <si>
-    <t>ifType</t>
-  </si>
-  <si>
-    <t>接口的类型</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.4</t>
-  </si>
-  <si>
-    <t>ifMtu</t>
-  </si>
-  <si>
-    <t>接口的最大传输单元</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.5</t>
-  </si>
-  <si>
-    <t>ifSpeed</t>
-  </si>
-  <si>
-    <t>接口的速率</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.6</t>
-  </si>
-  <si>
-    <t>ifPhysAddress</t>
-  </si>
-  <si>
-    <t>接口的物理地址</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.7</t>
-  </si>
-  <si>
-    <t>ifAdminStatus</t>
-  </si>
-  <si>
-    <t>接口的管理状态</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.8</t>
-  </si>
-  <si>
-    <t>ifOperStatus</t>
-  </si>
-  <si>
-    <t>接口的操作状态</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.9</t>
-  </si>
-  <si>
-    <t>ifLastChange</t>
-  </si>
-  <si>
-    <t>接口的最后修改时间</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.10</t>
-  </si>
-  <si>
-    <t>ifInOctets</t>
-  </si>
-  <si>
-    <t>接口接收的字节数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.11</t>
-  </si>
-  <si>
-    <t>ifInUcastPkts</t>
-  </si>
-  <si>
-    <t>接口接收的单播数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.12</t>
-  </si>
-  <si>
-    <t>ifInNUcastPkts</t>
-  </si>
-  <si>
-    <t>接口接收的非单播数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.13</t>
-  </si>
-  <si>
-    <t>ifInDiscards</t>
-  </si>
-  <si>
-    <t>接口接收的丢弃数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.14</t>
-  </si>
-  <si>
-    <t>ifInErrors</t>
-  </si>
-  <si>
-    <t>接口接收的错误数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.15</t>
-  </si>
-  <si>
-    <t>ifInUnknownProtos</t>
-  </si>
-  <si>
-    <t>接口接收的未知协议数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.16</t>
-  </si>
-  <si>
-    <t>ifOutOctets</t>
-  </si>
-  <si>
-    <t>接口发送的字节数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.17</t>
-  </si>
-  <si>
-    <t>ifOutUcastPkts</t>
-  </si>
-  <si>
-    <t>接口发送的单播数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.18</t>
-  </si>
-  <si>
-    <t>ifOutNUcastPkts</t>
-  </si>
-  <si>
-    <t>接口发送的非单播数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.19</t>
-  </si>
-  <si>
-    <t>ifOutDiscards</t>
-  </si>
-  <si>
-    <t>接口发送的丢弃数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.20</t>
-  </si>
-  <si>
-    <t>ifOutErrors</t>
-  </si>
-  <si>
-    <t>接口发送的错误数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.2.2.1.21</t>
-  </si>
-  <si>
-    <t>ifOutQLen</t>
-  </si>
-  <si>
-    <t>接口发送队列的长度</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.1</t>
-  </si>
-  <si>
-    <t>ipForwarding</t>
-  </si>
-  <si>
-    <t>IP 转发表的状态</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.2</t>
-  </si>
-  <si>
-    <t>ipDefaultTTL</t>
-  </si>
-  <si>
-    <t>IP 数据包的默认 TTL</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.3</t>
-  </si>
-  <si>
-    <t>ipInReceives</t>
-  </si>
-  <si>
-    <t>接收的 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.4</t>
-  </si>
-  <si>
-    <t>ipInHdrErrors</t>
-  </si>
-  <si>
-    <t>接收的 IP 包头错误数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.5</t>
-  </si>
-  <si>
-    <t>ipInAddrErrors</t>
-  </si>
-  <si>
-    <t>接收的 IP 地址错误数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.6</t>
-  </si>
-  <si>
-    <t>ipForwDatagrams</t>
-  </si>
-  <si>
-    <t>转发的 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.7</t>
-  </si>
-  <si>
-    <t>ipInUnknownProtos</t>
-  </si>
-  <si>
-    <t>接收的未知协议 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.8</t>
-  </si>
-  <si>
-    <t>ipInDiscards</t>
-  </si>
-  <si>
-    <t>接收的丢弃 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.9</t>
-  </si>
-  <si>
-    <t>ipInDelivers</t>
-  </si>
-  <si>
-    <t>接收并送达的 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.10</t>
-  </si>
-  <si>
-    <t>ipOutRequests</t>
-  </si>
-  <si>
-    <t>发送的 IP 请求包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.11</t>
-  </si>
-  <si>
-    <t>ipOutDiscards</t>
-  </si>
-  <si>
-    <t>发送的丢弃 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.12</t>
-  </si>
-  <si>
-    <t>ipOutNoRoutes</t>
-  </si>
-  <si>
-    <t>发送的无路由 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.13</t>
-  </si>
-  <si>
-    <t>ipReasmTimeout</t>
-  </si>
-  <si>
-    <t>IP 数据包重组超时数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.14</t>
-  </si>
-  <si>
-    <t>ipReasmReqds</t>
-  </si>
-  <si>
-    <t>IP 数据包重组请求数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.15</t>
-  </si>
-  <si>
-    <t>ipReasmOKs</t>
-  </si>
-  <si>
-    <t>成功重组的 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.16</t>
-  </si>
-  <si>
-    <t>ipReasmFails</t>
-  </si>
-  <si>
-    <t>重组失败的 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.17</t>
-  </si>
-  <si>
-    <t>ipFragOKs</t>
-  </si>
-  <si>
-    <t>成功分段的 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.18</t>
-  </si>
-  <si>
-    <t>ipFragFails</t>
-  </si>
-  <si>
-    <t>分段失败的 IP 数据包数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.3.1.19</t>
-  </si>
-  <si>
-    <t>ipFragCreates</t>
-  </si>
-  <si>
-    <t>创建的 IP 数据包分段数</t>
-  </si>
-  <si>
-    <t>1.3.6.1.2.1.4.1</t>
-  </si>
-  <si>
-    <t>icmpInMsgs</t>
-  </si>
-  <si>
-    <t>接收的 ICMP 消息数</t>
+    <t>.1.3.6.1.2.1.1.5.0</t>
+  </si>
+  <si>
+    <t>获取机器名</t>
+  </si>
+  <si>
+    <t>SysName</t>
+  </si>
+  <si>
+    <t>.1.3.6.1.2.1.1.6.0</t>
+  </si>
+  <si>
+    <t>机器坐在位置</t>
+  </si>
+  <si>
+    <t>SysLocation</t>
+  </si>
+  <si>
+    <t>.1.3.6.1.2.1.1.7.0</t>
+  </si>
+  <si>
+    <t>机器提供的服务</t>
+  </si>
+  <si>
+    <t>SysService</t>
+  </si>
+  <si>
+    <t>.1.3.6.1.2.1.2.1.0</t>
+  </si>
+  <si>
+    <t>网络接口的数目</t>
+  </si>
+  <si>
+    <t>IfNumber</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +746,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1133,6 +755,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1664,14 +1289,14 @@
   <sheetPr/>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="22.625" customWidth="1"/>
-    <col min="2" max="2" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="36.375" customWidth="1"/>
     <col min="3" max="3" width="27.75" customWidth="1"/>
     <col min="4" max="4" width="11.625" customWidth="1"/>
   </cols>
@@ -1789,592 +1414,256 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D43" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D49" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D50" s="3">
-        <v>1000</v>
-      </c>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>